<commit_message>
remove mandatory parameters. Can create story and task without description and priority
</commit_message>
<xml_diff>
--- a/JiraLoader/jiraLoader-core/src/test/resources/excelTestFiles/Import_JIRA_TEST1.xlsx
+++ b/JiraLoader/jiraLoader-core/src/test/resources/excelTestFiles/Import_JIRA_TEST1.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="24915" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Présentation" sheetId="4" r:id="rId1"/>
     <sheet name="Import" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:E18"/>
 </workbook>
 </file>
 
@@ -156,7 +157,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -686,8 +686,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -818,19 +818,19 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="74.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="46.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="74.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="46.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
CMO - Allowed to configure application via the first excel sheet - Added also a version number to the excel file. Required version number is 2 - Added the possibility to check if an story exists before to create it. In this case, the story is reused
</commit_message>
<xml_diff>
--- a/JiraLoader/jiraLoader-core/src/test/resources/excelTestFiles/Import_JIRA_TEST1.xlsx
+++ b/JiraLoader/jiraLoader-core/src/test/resources/excelTestFiles/Import_JIRA_TEST1.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6060" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Présentation" sheetId="4" r:id="rId1"/>
+    <sheet name="Configuration" sheetId="4" r:id="rId1"/>
     <sheet name="Import" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>Version</t>
   </si>
@@ -120,9 +119,6 @@
     <t>ODYSEE-Indus</t>
   </si>
   <si>
-    <t xml:space="preserve">UO de test pour Jira </t>
-  </si>
-  <si>
     <t>Hey, c'est mon UO de test</t>
   </si>
   <si>
@@ -151,13 +147,96 @@
   </si>
   <si>
     <t>1h</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Valeurs possibles</t>
+  </si>
+  <si>
+    <t>autoriser les mises à jours des tâches</t>
+  </si>
+  <si>
+    <t>Repercuter les mises à jours des tâches sur les sous taches</t>
+  </si>
+  <si>
+    <t>Commentaires</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Permet de mettre à jour la </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>priorité</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> d'une tache</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Permet de mettre à jour la </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>priorité</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> des sous taches d'une tâche lorsque que la tâche est mise à jour</t>
+    </r>
+  </si>
+  <si>
+    <t>Rechercher si une story existe déjà lors de la creation</t>
+  </si>
+  <si>
+    <t>Lors de la création d'une story, le programme va rechercher si une story possède le même DEBUT de nom. 
+Par exemple, si la story porte le nom "M5T_G01R12C06_BCA_KPSA_1048_1 | nouveau SDM round robin - fichiers de conf osdp.cfg", le programme va rechercher si une story commence avec le nom "M5T_G01R12C06_BCA_KPSA_1048_1". Si oui, celle ci sera récupérer et aucune story ne sera créé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5T_G01R12C06_BCA_KPSA_1048_1 | UO de test pour Jira </t>
+  </si>
+  <si>
+    <t>(true / false)</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +255,14 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -359,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -376,6 +463,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,19 +776,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="90.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
@@ -700,8 +801,18 @@
       <c r="C1" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="17"/>
+      <c r="G1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -711,8 +822,16 @@
       <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -722,8 +841,20 @@
       <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -733,8 +864,20 @@
       <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -744,64 +887,77 @@
       <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7" t="s">
         <v>30</v>
@@ -809,7 +965,11 @@
       <c r="C14" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -818,7 +978,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,7 +1024,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>0</v>
@@ -880,7 +1040,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
@@ -893,7 +1053,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -909,16 +1069,16 @@
         <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -934,19 +1094,19 @@
         <v>33</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -961,19 +1121,19 @@
         <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1082,13 +1242,13 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Présentation!$A$2:$A$14</xm:f>
+            <xm:f>Configuration!$A$2:$A$14</xm:f>
           </x14:formula1>
           <xm:sqref>B1:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Présentation!$C$2:$C$14</xm:f>
+            <xm:f>Configuration!$C$2:$C$14</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
CMO - fixng configuration file
</commit_message>
<xml_diff>
--- a/JiraLoader/jiraLoader-core/src/test/resources/excelTestFiles/Import_JIRA_TEST1.xlsx
+++ b/JiraLoader/jiraLoader-core/src/test/resources/excelTestFiles/Import_JIRA_TEST1.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16320" windowHeight="6990"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="4" r:id="rId1"/>
     <sheet name="Import" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:G17"/>
 </workbook>
 </file>
 
@@ -156,9 +157,6 @@
   </si>
   <si>
     <t>autoriser les mises à jours des tâches</t>
-  </si>
-  <si>
-    <t>Repercuter les mises à jours des tâches sur les sous taches</t>
   </si>
   <si>
     <t>Commentaires</t>
@@ -219,17 +217,20 @@
     <t>Rechercher si une story existe déjà lors de la creation</t>
   </si>
   <si>
+    <t xml:space="preserve">M5T_G01R12C06_BCA_KPSA_1048_1 | UO de test pour Jira </t>
+  </si>
+  <si>
+    <t>(true / false)</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
     <t>Lors de la création d'une story, le programme va rechercher si une story possède le même DEBUT de nom. 
-Par exemple, si la story porte le nom "M5T_G01R12C06_BCA_KPSA_1048_1 | nouveau SDM round robin - fichiers de conf osdp.cfg", le programme va rechercher si une story commence avec le nom "M5T_G01R12C06_BCA_KPSA_1048_1". Si oui, celle ci sera récupérer et aucune story ne sera créé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M5T_G01R12C06_BCA_KPSA_1048_1 | UO de test pour Jira </t>
-  </si>
-  <si>
-    <t>(true / false)</t>
-  </si>
-  <si>
-    <t>false</t>
+Par exemple, si la story porte le nom "M5T_G01R12C06_BCA_KPSA_1048_1 | nouveau SDM round robin - fichiers de conf osdp.cfg", le programme va rechercher si une story commence avec le nom "M5T_G01R12C06_BCA_KPSA_1048_1". Si oui, celle ci sera récupérée et aucune story ne sera créée</t>
+  </si>
+  <si>
+    <t>Repercuter les mises à jours des sous-taches d'une tâche</t>
   </si>
 </sst>
 </file>
@@ -778,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +810,7 @@
         <v>45</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -842,16 +843,16 @@
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="16" t="s">
         <v>54</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -868,13 +869,13 @@
         <v>46</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -888,16 +889,16 @@
         <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -977,7 +978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1069,7 +1070,7 @@
         <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>34</v>

</xml_diff>